<commit_message>
more fixes with Inho
</commit_message>
<xml_diff>
--- a/code/roster.xlsx
+++ b/code/roster.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,60 +436,50 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>term_code</t>
+          <t>person_name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>term_name</t>
+          <t>person_email</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>person_name</t>
+          <t>person_eid</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>person_email</t>
+          <t>person_vid</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>person_eid</t>
+          <t>person_role</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>person_vid</t>
+          <t>person_github_id</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>person_role</t>
+          <t>person_headshot</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>person_github_id</t>
+          <t>person_linkedin</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>person_headshot</t>
+          <t>person_portfolio</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>person_linkedin</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>person_portfolio</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>person_orcid</t>
         </is>
@@ -498,56 +488,46 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>John Leonard</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>jdleonard@vcu.edu</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>John Leonard</t>
+          <t>jdleonard</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>jdleonard@vcu.edu</t>
+          <t>V00758858</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>jdleonard</t>
+          <t>Faculty Mentor</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>V00758858</t>
+          <t>jleonard99</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Faculty Mentor</t>
+          <t>jdleonard-2.jpg</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>jleonard99</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>jdleonard-2.jpg</t>
-        </is>
-      </c>
+          <t>https://www.linkedin.com/in/johndleonard/</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/johndleonard/</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
         <is>
           <t>https://orcid.org/0000-0002-1871-3178</t>
         </is>
@@ -556,344 +536,294 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>William Benton</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>wbenton@vcu.edu</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>William Benton</t>
+          <t>wbenton</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>wbenton@vcu.edu</t>
+          <t>V00852704</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>wbenton</t>
+          <t>Faculty Mentor</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>V00852704</t>
+          <t>wbenton1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Faculty Mentor</t>
+          <t>wbenton.jpg</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>wbenton1</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>wbenton.jpg</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
           <t>https://www.linkedin.com/in/williambenton1/</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>Sneha Dasari</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>dasariss@vcu.edu</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sneha Dasari</t>
+          <t>dasariss</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>dasariss@vcu.edu</t>
+          <t>V00946443</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>dasariss</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>V00946443</t>
-        </is>
-      </c>
+          <t>Current Student</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Current Student</t>
+          <t>dasariss.png</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>dasariss.png</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>Javeria Hanif</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>hanifj@vcu.edu</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Javeria Hanif</t>
+          <t>hanifj</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>hanifj@vcu.edu</t>
+          <t>V01009229</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>hanifj</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>V01009229</t>
-        </is>
-      </c>
+          <t>Current Student</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Current Student</t>
+          <t>hanifj.png</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>hanifj.png</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>Mallika Lakshminarayan</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>lakshminam@vcu.edu</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mallika Lakshminarayan</t>
+          <t>lakshminam</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>lakshminam@vcu.edu</t>
+          <t>V00955103</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>lakshminam</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>V00955103</t>
-        </is>
-      </c>
+          <t>Current Student</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Current Student</t>
+          <t>lakshminam.png</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>lakshminam.png</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>Rachel Nguyen</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>nguyenrm2@vcu.edu</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Rachel Nguyen</t>
+          <t>nguyenrm2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>nguyenrm2@vcu.edu</t>
+          <t>V00947809</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>nguyenrm2</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>V00947809</t>
-        </is>
-      </c>
+          <t>Current Student</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Current Student</t>
+          <t>nguyenrm2.png</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nguyenrm2.png</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>Inho Park</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>parki2@vcu.edu</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Inho Park</t>
+          <t>parki2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>parki2@vcu.edu</t>
+          <t>V00866161</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>parki2</t>
+          <t>Current Student</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>V00866161</t>
+          <t>inoxprk</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Current Student</t>
+          <t>parki2.png</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>inoxprk</t>
+          <t>www.linkedin.com/in/inhoprk</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>parki2.png</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>www.linkedin.com/in/inhoprk</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
           <t>https://www.inhodesign.com/</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>202410</t>
+          <t>Paul Reid</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Fall 2023</t>
+          <t>reidp@vcu.edu</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Paul Reid</t>
+          <t>reidp</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>reidp@vcu.edu</t>
+          <t>V01011857</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>reidp</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>V01011857</t>
-        </is>
-      </c>
+          <t>Current Student</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Current Student</t>
+          <t>reidp.png</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>reidp.png</t>
-        </is>
-      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kian</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Alumni</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>